<commit_message>
Updated paper and Results file
</commit_message>
<xml_diff>
--- a/Report/Results.xlsx
+++ b/Report/Results.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
   <si>
     <t>Elements</t>
   </si>
@@ -34,6 +35,9 @@
   </si>
   <si>
     <t>Speedup</t>
+  </si>
+  <si>
+    <t>MultiGPU</t>
   </si>
 </sst>
 </file>
@@ -287,25 +291,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="86780160"/>
-        <c:axId val="86794240"/>
+        <c:axId val="73675904"/>
+        <c:axId val="73677440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86780160"/>
+        <c:axId val="73675904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86794240"/>
+        <c:crossAx val="73677440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86794240"/>
+        <c:axId val="73677440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,7 +317,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86780160"/>
+        <c:crossAx val="73675904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -326,7 +330,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -336,9 +340,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -348,7 +349,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -410,7 +411,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$14</c:f>
+              <c:f>Sheet1!$F$2:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -457,26 +458,92 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MultiGPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$1:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12294585238634027</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.46456517095722516</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2218592607079992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8426278845080448</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5518256151878189</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.528953278578836</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.988656436678788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="67314048"/>
-        <c:axId val="67315584"/>
+        <c:axId val="73684864"/>
+        <c:axId val="73686400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67314048"/>
+        <c:axId val="73684864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67315584"/>
+        <c:crossAx val="73686400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67315584"/>
+        <c:axId val="73686400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +551,187 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67314048"/>
+        <c:crossAx val="73684864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parallel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$8:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>131072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$8:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>325096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1379843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5743033</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23653931</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96906222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>394990289</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1603625399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MultiGPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$8:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4990026</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5262252</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6391250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11000316</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29873519</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>106874874</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>415907759</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="81328000"/>
+        <c:axId val="81329536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="81328000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81329536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="81329536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81328000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -507,16 +754,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -537,16 +784,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -560,6 +807,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -853,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -865,9 +1142,10 @@
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -881,10 +1159,13 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>32</v>
       </c>
@@ -897,12 +1178,16 @@
       <c r="D2">
         <v>621</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E14" si="0">C2/D2</f>
+      <c r="F2">
+        <f>C2/D2</f>
         <v>4.4460547504025767</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" t="e">
+        <f>C2/E2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>64</v>
       </c>
@@ -915,12 +1200,16 @@
       <c r="D3">
         <v>751</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="F3">
+        <f>C3/D3</f>
         <v>4.1824234354194409</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" t="e">
+        <f t="shared" ref="G3:G14" si="0">C3/E3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>128</v>
       </c>
@@ -933,12 +1222,16 @@
       <c r="D4">
         <v>1563</v>
       </c>
-      <c r="E4">
+      <c r="F4">
+        <f>C4/D4</f>
+        <v>3.0236724248240563</v>
+      </c>
+      <c r="G4" t="e">
         <f t="shared" si="0"/>
-        <v>3.0236724248240563</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>256</v>
       </c>
@@ -951,12 +1244,16 @@
       <c r="D5">
         <v>4637</v>
       </c>
-      <c r="E5">
+      <c r="F5">
+        <f>C5/D5</f>
+        <v>2.372439076989433</v>
+      </c>
+      <c r="G5" t="e">
         <f t="shared" si="0"/>
-        <v>2.372439076989433</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>512</v>
       </c>
@@ -969,12 +1266,16 @@
       <c r="D6">
         <v>17614</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <f>C6/D6</f>
+        <v>2.0669921653230383</v>
+      </c>
+      <c r="G6" t="e">
         <f t="shared" si="0"/>
-        <v>2.0669921653230383</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>1024</v>
       </c>
@@ -987,12 +1288,16 @@
       <c r="D7">
         <v>75415</v>
       </c>
-      <c r="E7">
+      <c r="F7">
+        <f>C7/D7</f>
+        <v>1.9224292249552477</v>
+      </c>
+      <c r="G7" t="e">
         <f t="shared" si="0"/>
-        <v>1.9224292249552477</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>2048</v>
       </c>
@@ -1006,11 +1311,18 @@
         <v>325096</v>
       </c>
       <c r="E8">
+        <v>4990026</v>
+      </c>
+      <c r="F8">
+        <f>C8/D8</f>
+        <v>1.8871441051258706</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>1.8871441051258706</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.12294585238634027</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>4096</v>
       </c>
@@ -1024,11 +1336,18 @@
         <v>1379843</v>
       </c>
       <c r="E9">
+        <v>5262252</v>
+      </c>
+      <c r="F9">
+        <f>C9/D9</f>
+        <v>1.7716935912274077</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>1.7716935912274077</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>0.46456517095722516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8192</v>
       </c>
@@ -1039,11 +1358,18 @@
         <v>5743033</v>
       </c>
       <c r="E10">
+        <v>6391250</v>
+      </c>
+      <c r="F10">
+        <f>C10/D10</f>
+        <v>1.3597706995589265</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
-        <v>1.3597706995589265</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1.2218592607079992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>16384</v>
       </c>
@@ -1054,11 +1380,18 @@
         <v>23653931</v>
       </c>
       <c r="E11">
+        <v>11000316</v>
+      </c>
+      <c r="F11">
+        <f>C11/D11</f>
+        <v>1.3219707540366123</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>1.3219707540366123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>2.8426278845080448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>32768</v>
       </c>
@@ -1069,11 +1402,18 @@
         <v>96906222</v>
       </c>
       <c r="E12">
+        <v>29873519</v>
+      </c>
+      <c r="F12">
+        <f>C12/D12</f>
+        <v>1.4032024589711072</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>1.4032024589711072</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>4.5518256151878189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>65536</v>
       </c>
@@ -1084,11 +1424,18 @@
         <v>394990289</v>
       </c>
       <c r="E13">
+        <v>106874874</v>
+      </c>
+      <c r="F13">
+        <f>C13/D13</f>
+        <v>1.766577757561022</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>1.766577757561022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>6.528953278578836</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>131072</v>
       </c>
@@ -1099,8 +1446,15 @@
         <v>1603625399</v>
       </c>
       <c r="E14">
+        <v>415907759</v>
+      </c>
+      <c r="F14">
+        <f>C14/D14</f>
+        <v>1.5531860991682884</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
-        <v>1.5531860991682884</v>
+        <v>5.988656436678788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on the paper and results
</commit_message>
<xml_diff>
--- a/Report/Results.xlsx
+++ b/Report/Results.xlsx
@@ -17,12 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="8">
   <si>
     <t>Elements</t>
-  </si>
-  <si>
-    <t>Cuda Time (usec)</t>
   </si>
   <si>
     <t>SNAP</t>
@@ -31,13 +28,19 @@
     <t>x</t>
   </si>
   <si>
-    <t>Parallel</t>
-  </si>
-  <si>
     <t>Speedup</t>
   </si>
   <si>
-    <t>MultiGPU</t>
+    <t>Vertex</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>MPI</t>
+  </si>
+  <si>
+    <t>Edge Discovery</t>
   </si>
 </sst>
 </file>
@@ -97,11 +100,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cuda Time (usec)</c:v>
+                  <c:v>Vertex</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -111,7 +114,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -150,7 +153,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Sheet1!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -196,7 +199,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -210,7 +213,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -249,7 +252,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>Sheet1!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -349,7 +352,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -363,7 +366,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$3:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -411,7 +414,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$14</c:f>
+              <c:f>Sheet1!$G$3:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -463,11 +466,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MultiGPU</c:v>
+                  <c:v>MPI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -477,26 +480,11 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$1:$G$14</c:f>
+              <c:f>Sheet1!$H$2:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
@@ -583,11 +571,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Parallel</c:v>
+                  <c:v>Edge Discovery</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -597,7 +585,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$8:$A$14</c:f>
+              <c:f>Sheet1!$A$9:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -627,7 +615,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$8:$D$14</c:f>
+              <c:f>Sheet1!$D$9:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -661,11 +649,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MultiGPU</c:v>
+                  <c:v>MPI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -675,7 +663,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$8:$E$14</c:f>
+              <c:f>Sheet1!$E$9:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -754,15 +742,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -784,15 +772,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -816,13 +804,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1130,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1142,318 +1130,337 @@
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="5" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
         <v>32</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>6578</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>2761</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>621</v>
       </c>
-      <c r="F2">
-        <f>C2/D2</f>
+      <c r="F3">
+        <f>C3/B3</f>
+        <v>0.4197324414715719</v>
+      </c>
+      <c r="G3">
+        <f>C3/D3</f>
         <v>4.4460547504025767</v>
       </c>
-      <c r="G2" t="e">
-        <f>C2/E2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
         <v>64</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>18334</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>3141</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>751</v>
       </c>
-      <c r="F3">
-        <f>C3/D3</f>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="0">C4/B4</f>
+        <v>0.17132104287116831</v>
+      </c>
+      <c r="G4">
+        <f>C4/D4</f>
         <v>4.1824234354194409</v>
       </c>
-      <c r="G3" t="e">
-        <f t="shared" ref="G3:G14" si="0">C3/E3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
         <v>128</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>63658</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>4726</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>1563</v>
       </c>
-      <c r="F4">
-        <f>C4/D4</f>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>7.4240472525055765E-2</v>
+      </c>
+      <c r="G5">
+        <f>C5/D5</f>
         <v>3.0236724248240563</v>
       </c>
-      <c r="G4" t="e">
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>256</v>
+      </c>
+      <c r="B6">
+        <v>235117</v>
+      </c>
+      <c r="C6">
+        <v>11001</v>
+      </c>
+      <c r="D6">
+        <v>4637</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>256</v>
-      </c>
-      <c r="B5">
-        <v>235117</v>
-      </c>
-      <c r="C5">
-        <v>11001</v>
-      </c>
-      <c r="D5">
-        <v>4637</v>
-      </c>
-      <c r="F5">
-        <f>C5/D5</f>
+        <v>4.6789470774125222E-2</v>
+      </c>
+      <c r="G6">
+        <f>C6/D6</f>
         <v>2.372439076989433</v>
       </c>
-      <c r="G5" t="e">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>512</v>
+      </c>
+      <c r="B7">
+        <v>877849</v>
+      </c>
+      <c r="C7">
+        <v>36408</v>
+      </c>
+      <c r="D7">
+        <v>17614</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>512</v>
-      </c>
-      <c r="B6">
-        <v>877849</v>
-      </c>
-      <c r="C6">
-        <v>36408</v>
-      </c>
-      <c r="D6">
-        <v>17614</v>
-      </c>
-      <c r="F6">
-        <f>C6/D6</f>
+        <v>4.14741031771979E-2</v>
+      </c>
+      <c r="G7">
+        <f>C7/D7</f>
         <v>2.0669921653230383</v>
       </c>
-      <c r="G6" t="e">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>1024</v>
+      </c>
+      <c r="B8">
+        <v>3488531</v>
+      </c>
+      <c r="C8">
+        <v>144980</v>
+      </c>
+      <c r="D8">
+        <v>75415</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>1024</v>
-      </c>
-      <c r="B7">
-        <v>3488531</v>
-      </c>
-      <c r="C7">
-        <v>144980</v>
-      </c>
-      <c r="D7">
-        <v>75415</v>
-      </c>
-      <c r="F7">
-        <f>C7/D7</f>
+        <v>4.1559040180522977E-2</v>
+      </c>
+      <c r="G8">
+        <f>C8/D8</f>
         <v>1.9224292249552477</v>
       </c>
-      <c r="G7" t="e">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>2048</v>
+      </c>
+      <c r="B9">
+        <v>14091411</v>
+      </c>
+      <c r="C9">
+        <v>613503</v>
+      </c>
+      <c r="D9">
+        <v>325096</v>
+      </c>
+      <c r="E9">
+        <v>4990026</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>2048</v>
-      </c>
-      <c r="B8">
-        <v>14091411</v>
-      </c>
-      <c r="C8">
-        <v>613503</v>
-      </c>
-      <c r="D8">
-        <v>325096</v>
-      </c>
-      <c r="E8">
-        <v>4990026</v>
-      </c>
-      <c r="F8">
-        <f>C8/D8</f>
+        <v>4.3537371807550004E-2</v>
+      </c>
+      <c r="G9">
+        <f>C9/D9</f>
         <v>1.8871441051258706</v>
       </c>
-      <c r="G8">
+      <c r="H9">
+        <f t="shared" ref="H4:H15" si="1">C9/E9</f>
+        <v>0.12294585238634027</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>4096</v>
+      </c>
+      <c r="B10">
+        <v>58778463</v>
+      </c>
+      <c r="C10">
+        <v>2444659</v>
+      </c>
+      <c r="D10">
+        <v>1379843</v>
+      </c>
+      <c r="E10">
+        <v>5262252</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
-        <v>0.12294585238634027</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>4096</v>
-      </c>
-      <c r="B9">
-        <v>58778463</v>
-      </c>
-      <c r="C9">
-        <v>2444659</v>
-      </c>
-      <c r="D9">
-        <v>1379843</v>
-      </c>
-      <c r="E9">
-        <v>5262252</v>
-      </c>
-      <c r="F9">
-        <f>C9/D9</f>
+        <v>4.1591067122663618E-2</v>
+      </c>
+      <c r="G10">
+        <f>C10/D10</f>
         <v>1.7716935912274077</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
+      <c r="H10">
+        <f t="shared" si="1"/>
         <v>0.46456517095722516</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
+    <row r="11" spans="1:8">
+      <c r="A11">
         <v>8192</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>7809208</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>5743033</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>6391250</v>
       </c>
-      <c r="F10">
-        <f>C10/D10</f>
+      <c r="G11">
+        <f>C11/D11</f>
         <v>1.3597706995589265</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
+      <c r="H11">
+        <f t="shared" si="1"/>
         <v>1.2218592607079992</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
+    <row r="12" spans="1:8">
+      <c r="A12">
         <v>16384</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>31269805</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>23653931</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>11000316</v>
       </c>
-      <c r="F11">
-        <f>C11/D11</f>
+      <c r="G12">
+        <f>C12/D12</f>
         <v>1.3219707540366123</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
+      <c r="H12">
+        <f t="shared" si="1"/>
         <v>2.8426278845080448</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
+    <row r="13" spans="1:8">
+      <c r="A13">
         <v>32768</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>135979049</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>96906222</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>29873519</v>
       </c>
-      <c r="F12">
-        <f>C12/D12</f>
+      <c r="G13">
+        <f>C13/D13</f>
         <v>1.4032024589711072</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
+      <c r="H13">
+        <f t="shared" si="1"/>
         <v>4.5518256151878189</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
+    <row r="14" spans="1:8">
+      <c r="A14">
         <v>65536</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>697781059</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>394990289</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>106874874</v>
       </c>
-      <c r="F13">
-        <f>C13/D13</f>
+      <c r="G14">
+        <f>C14/D14</f>
         <v>1.766577757561022</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
+      <c r="H14">
+        <f t="shared" si="1"/>
         <v>6.528953278578836</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
+    <row r="15" spans="1:8">
+      <c r="A15">
         <v>131072</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>2490728678</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>1603625399</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>415907759</v>
       </c>
-      <c r="F14">
-        <f>C14/D14</f>
+      <c r="G15">
+        <f>C15/D15</f>
         <v>1.5531860991682884</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
+      <c r="H15">
+        <f t="shared" si="1"/>
         <v>5.988656436678788</v>
       </c>
     </row>
@@ -1510,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1518,28 +1525,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1547,10 +1554,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1558,13 +1565,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1572,13 +1579,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1586,13 +1593,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1600,13 +1607,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1614,13 +1621,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1628,10 +1635,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1639,22 +1646,22 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the report
</commit_message>
<xml_diff>
--- a/Report/Results.xlsx
+++ b/Report/Results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="7">
   <si>
     <t>Elements</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Vertex</t>
-  </si>
-  <si>
-    <t>Edge</t>
   </si>
   <si>
     <t>MPI</t>
@@ -91,6 +88,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Running Time Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -100,11 +115,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Sheet1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Vertex</c:v>
+                  <c:v>Edge Discovery</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -114,10 +129,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>(Sheet1!$A$3:$A$12,Sheet1!$A$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
@@ -147,6 +162,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -213,10 +231,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>(Sheet1!$A$3:$A$12,Sheet1!$A$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
@@ -246,6 +264,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -303,6 +324,24 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Graph Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="73677440"/>
@@ -318,6 +357,29 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Running</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (usec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="73675904"/>
@@ -343,6 +405,29 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speedup Relative</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> to SNAP</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -352,11 +437,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Speedup</c:v>
+                  <c:v>Edge Discovery</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -480,32 +565,29 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$15</c:f>
+              <c:f>Sheet1!$H$3:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="13"/>
+                <c:pt idx="6">
+                  <c:v>0.12294585238634027</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.12294585238634027</c:v>
+                  <c:v>0.46456517095722516</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46456517095722516</c:v>
+                  <c:v>1.2218592607079992</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2218592607079992</c:v>
+                  <c:v>2.8426278845080448</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8426278845080448</c:v>
+                  <c:v>4.5518256151878189</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.5518256151878189</c:v>
+                  <c:v>6.528953278578836</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.528953278578836</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>5.988656436678788</c:v>
                 </c:pt>
               </c:numCache>
@@ -522,6 +604,24 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Graph Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="73686400"/>
@@ -537,6 +637,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="73684864"/>
@@ -562,6 +680,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Running Time Comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -702,6 +839,24 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Graph Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="81329536"/>
@@ -717,6 +872,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Running Time (usec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="81328000"/>
@@ -772,16 +945,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -803,15 +976,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>200026</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1120,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1131,6 +1304,7 @@
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1149,19 +1323,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>